<commit_message>
Made the code much more functional and easier to read
</commit_message>
<xml_diff>
--- a/src/main/Book1.xlsx
+++ b/src/main/Book1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hensoro\IdeaProjects\Friendship\src\main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hensoro\Documents\Collab-Projects\Friendship\src\main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1074F8A6-3E4F-46EB-9B22-E0F29D32EB46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C580130E-636F-4BD4-B3ED-4A902B22F12A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1F63989F-E1AE-47CB-9EA1-BCEE5DF6253B}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{1F63989F-E1AE-47CB-9EA1-BCEE5DF6253B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>Kiss me</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>rawr</t>
+  </si>
+  <si>
+    <t>Movie 6</t>
   </si>
 </sst>
 </file>
@@ -512,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB6E04D4-C071-4E7C-A65A-7003BC014941}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,19 +546,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -665,6 +674,29 @@
       </c>
       <c r="G6" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>